<commit_message>
some concept bug fixes
</commit_message>
<xml_diff>
--- a/concepts/technologies-br-mitigation-br/input.xlsx
+++ b/concepts/technologies-br-mitigation-br/input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalyan/Documents/CPR/global-stocktake/concepts/technologies-br-mitigation-br/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01028FA-BD23-D745-B85C-8E1896AC5017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF83BA21-66C2-6E4C-A9AC-79A98A6165B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="396">
   <si>
     <t>Pattern name (optional)</t>
   </si>
@@ -1158,6 +1158,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> For any rules ending in _</t>
@@ -1176,6 +1177,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, values should be comma-separated. </t>
@@ -1265,7 +1267,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1327,6 +1329,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1385,14 +1394,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1615,8 +1624,8 @@
   </sheetPr>
   <dimension ref="A1:AT210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157:B161"/>
+    <sheetView tabSelected="1" topLeftCell="C167" workbookViewId="0">
+      <selection activeCell="F201" sqref="F201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1630,16 +1639,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
@@ -1672,19 +1681,19 @@
       <c r="V1" s="11"/>
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="Z1" s="11"/>
       <c r="AA1" s="11"/>
       <c r="AB1" s="11"/>
-      <c r="AC1" s="12" t="s">
+      <c r="AC1" s="14" t="s">
         <v>10</v>
       </c>
       <c r="AD1" s="11"/>
       <c r="AE1" s="11"/>
       <c r="AF1" s="11"/>
-      <c r="AG1" s="12" t="s">
+      <c r="AG1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="AH1" s="11"/>
@@ -8400,7 +8409,9 @@
       <c r="D120" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E120" s="6"/>
+      <c r="E120" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="F120" s="6" t="s">
         <v>172</v>
       </c>
@@ -13598,6 +13609,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="A1:A2"/>
@@ -13605,11 +13621,6 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:H1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AJ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>